<commit_message>
added popular tricks data
</commit_message>
<xml_diff>
--- a/data/Tricking Data Visualization Project Survey (Responses).xlsx
+++ b/data/Tricking Data Visualization Project Survey (Responses).xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mikael/Documents/TrickingData/data/"/>
@@ -15,17 +15,16 @@
     <sheet name="Gender" sheetId="4" r:id="rId1"/>
     <sheet name="Discovery to Number of Years" sheetId="8" r:id="rId2"/>
     <sheet name="Sheet9" sheetId="10" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="12" r:id="rId5"/>
-    <sheet name="Form Responses 1" sheetId="1" r:id="rId6"/>
-    <sheet name="Most Popular Tricks" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="12" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId5"/>
+    <sheet name="Most Popular Tricks" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Form Responses 1'!$A$1:$P$327</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Form Responses 1'!$A$1:$P$327</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId8"/>
+    <pivotCache cacheId="10" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4407" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4421" uniqueCount="1273">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3852,6 +3851,9 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>Overall</t>
   </si>
 </sst>
 </file>
@@ -12865,285 +12867,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:H29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="115.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5" customWidth="1"/>
-    <col min="4" max="4" width="3.83203125" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5" customWidth="1"/>
-    <col min="7" max="7" width="4.5" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13667,11 +13394,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J318" sqref="J318"/>
     </sheetView>
@@ -28217,12 +27944,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -28232,9 +27959,10 @@
     <col min="5" max="5" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>1219</v>
       </c>
@@ -28259,8 +27987,14 @@
       <c r="K1" s="14" t="s">
         <v>1220</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1267</v>
       </c>
@@ -28285,8 +28019,14 @@
       <c r="K2">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>540</v>
       </c>
@@ -28311,8 +28051,14 @@
       <c r="K3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M3" t="s">
+        <v>436</v>
+      </c>
+      <c r="N3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>534</v>
       </c>
@@ -28337,8 +28083,14 @@
       <c r="K4" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M4" t="s">
+        <v>158</v>
+      </c>
+      <c r="N4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>1221</v>
       </c>
@@ -28363,8 +28115,14 @@
       <c r="K5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M5">
+        <v>540</v>
+      </c>
+      <c r="N5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -28389,8 +28147,14 @@
       <c r="K6" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M6" t="s">
+        <v>534</v>
+      </c>
+      <c r="N6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -28415,8 +28179,14 @@
       <c r="K7" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M7" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>1222</v>
       </c>
@@ -28441,8 +28211,14 @@
       <c r="K8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M8" t="s">
+        <v>1234</v>
+      </c>
+      <c r="N8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>1254</v>
       </c>
@@ -28467,8 +28243,14 @@
       <c r="K9" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M9" t="s">
+        <v>232</v>
+      </c>
+      <c r="N9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>577</v>
       </c>
@@ -28493,8 +28275,14 @@
       <c r="K10" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M10" t="s">
+        <v>1247</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" s="11" t="s">
         <v>1223</v>
       </c>
@@ -28519,8 +28307,14 @@
       <c r="K11" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M11" t="s">
+        <v>449</v>
+      </c>
+      <c r="N11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
         <v>1224</v>
       </c>
@@ -28545,8 +28339,14 @@
       <c r="K12" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M12" t="s">
+        <v>372</v>
+      </c>
+      <c r="N12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" s="11" t="s">
         <v>1225</v>
       </c>
@@ -28571,8 +28371,14 @@
       <c r="K13" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M13" t="s">
+        <v>190</v>
+      </c>
+      <c r="N13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
         <v>145</v>
       </c>
@@ -28591,8 +28397,14 @@
       <c r="H14" s="9">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M14" t="s">
+        <v>477</v>
+      </c>
+      <c r="N14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
         <v>1246</v>
       </c>
@@ -28612,7 +28424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A16" s="11" t="s">
         <v>1247</v>
       </c>

</xml_diff>

<commit_message>
Fixed google trends data not showing up, hopefully
</commit_message>
<xml_diff>
--- a/data/Tricking Data Visualization Project Survey (Responses).xlsx
+++ b/data/Tricking Data Visualization Project Survey (Responses).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="4" r:id="rId1"/>
@@ -17,14 +17,16 @@
     <sheet name="Sheet9" sheetId="10" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="12" r:id="rId4"/>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId5"/>
-    <sheet name="Most Popular Tricks" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="14" r:id="rId7"/>
+    <sheet name="Most Popular Tricks" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Form Responses 1'!$A$1:$P$327</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4421" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4814" uniqueCount="1273">
   <si>
     <t>Timestamp</t>
   </si>
@@ -3990,7 +3992,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4593,11 +4594,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2092705856"/>
-        <c:axId val="-2117830368"/>
+        <c:axId val="2116234592"/>
+        <c:axId val="-2102208928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2092705856"/>
+        <c:axId val="2116234592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4640,7 +4641,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117830368"/>
+        <c:crossAx val="-2102208928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4648,7 +4649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117830368"/>
+        <c:axId val="-2102208928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4699,7 +4700,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2092705856"/>
+        <c:crossAx val="2116234592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4713,7 +4714,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11420,7 +11420,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="164" showAll="0"/>
@@ -11480,7 +11480,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="164" showAll="0"/>
@@ -11616,7 +11616,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="164" showAll="0"/>
@@ -11752,7 +11752,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="164" showAll="0"/>
@@ -13398,9 +13398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P327"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J318" sqref="J318"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A317" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2:N327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -27946,9 +27946,2071 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A181"/>
+  <sheetViews>
+    <sheetView topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A29" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A30" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A45" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A46" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A47" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A48" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A50" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A51" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A52" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A53" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A54" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A55" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A56" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A57" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A58" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A59" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A60" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A61" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A62" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A63" s="3" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A64" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A65" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A66" s="3" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A67" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A68" s="3" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A69" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A70" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A71" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A72" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A73" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A74" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A75" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A76" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A77" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A78" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A79" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A80" s="3" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A81" s="3" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A82" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A83" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A84" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A85" s="2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A86" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A87" s="2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A88" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A89" s="2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A90" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A91" s="2" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A92" s="3" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A93" s="2" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A94" s="3" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A95" s="3" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A96" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A97" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A98" s="2" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A99" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A100" s="2" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A101" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A102" s="2" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A103" s="2" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A104" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A105" s="2" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A106" s="2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A107" s="2" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A108" s="2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A109" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A110" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A111" s="2" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A112" s="3" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A113" s="3" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A114" s="2" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A115" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A116" s="2" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A117" s="2" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A118" s="2" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A119" s="2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A120" s="3" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A121" s="2" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A122" s="2" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A123" s="2" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A124" s="2" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A125" s="2" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A126" s="2" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A127" s="3" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A128" s="2" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A129" s="2" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A130" s="2" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A131" s="2" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A132" s="2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A133" s="2" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A134" s="2" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A135" s="2" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A136" s="2" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A137" s="3" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A138" s="2" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A139" s="2" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A140" s="2" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A141" s="2" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A142" s="2" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A143" s="2" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A144" s="2" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A145" s="2" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A146" s="2" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A147" s="2" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A148" s="3" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A149" s="2" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A150" s="3" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A151" s="2" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A152" s="2" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A153" s="2" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A154" s="2" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A155" s="2" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A156" s="3" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A157" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A158" s="2" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A159" s="2" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A160" s="2" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A161" s="3" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A162" s="3" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A163" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A164" s="3" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A165" s="2" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A166" s="2" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A167" s="2" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A168" s="2" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A169" s="2" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A170" s="2" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A171" s="2" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A172" s="3" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A173" s="3" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A174" s="3" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A175" s="3" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A176" s="3" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A177" s="3" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A178" s="3" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A179" s="3" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A180" s="2" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A181" s="3" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1"/>
+    <hyperlink ref="A17" r:id="rId2"/>
+    <hyperlink ref="A18" r:id="rId3"/>
+    <hyperlink ref="A20" r:id="rId4"/>
+    <hyperlink ref="A22" r:id="rId5"/>
+    <hyperlink ref="A36" r:id="rId6"/>
+    <hyperlink ref="A37" r:id="rId7"/>
+    <hyperlink ref="A38" r:id="rId8"/>
+    <hyperlink ref="A39" r:id="rId9"/>
+    <hyperlink ref="A48" r:id="rId10"/>
+    <hyperlink ref="A50" r:id="rId11"/>
+    <hyperlink ref="A51" r:id="rId12"/>
+    <hyperlink ref="A53" r:id="rId13"/>
+    <hyperlink ref="A55" r:id="rId14"/>
+    <hyperlink ref="A57" r:id="rId15"/>
+    <hyperlink ref="A58" r:id="rId16"/>
+    <hyperlink ref="A59" r:id="rId17"/>
+    <hyperlink ref="A61" r:id="rId18"/>
+    <hyperlink ref="A63" r:id="rId19"/>
+    <hyperlink ref="A66" r:id="rId20"/>
+    <hyperlink ref="A68" r:id="rId21"/>
+    <hyperlink ref="A80" r:id="rId22"/>
+    <hyperlink ref="A81" r:id="rId23"/>
+    <hyperlink ref="A92" r:id="rId24"/>
+    <hyperlink ref="A94" r:id="rId25"/>
+    <hyperlink ref="A95" r:id="rId26"/>
+    <hyperlink ref="A97" r:id="rId27"/>
+    <hyperlink ref="A112" r:id="rId28"/>
+    <hyperlink ref="A113" r:id="rId29"/>
+    <hyperlink ref="A120" r:id="rId30"/>
+    <hyperlink ref="A127" r:id="rId31"/>
+    <hyperlink ref="A137" r:id="rId32"/>
+    <hyperlink ref="A148" r:id="rId33"/>
+    <hyperlink ref="A150" r:id="rId34"/>
+    <hyperlink ref="A156" r:id="rId35"/>
+    <hyperlink ref="A161" r:id="rId36"/>
+    <hyperlink ref="A162" r:id="rId37"/>
+    <hyperlink ref="A164" r:id="rId38"/>
+    <hyperlink ref="A172" r:id="rId39"/>
+    <hyperlink ref="A173" r:id="rId40"/>
+    <hyperlink ref="A174" r:id="rId41"/>
+    <hyperlink ref="A175" r:id="rId42"/>
+    <hyperlink ref="A176" r:id="rId43"/>
+    <hyperlink ref="A177" r:id="rId44"/>
+    <hyperlink ref="A178" r:id="rId45"/>
+    <hyperlink ref="A179" r:id="rId46"/>
+    <hyperlink ref="A181" r:id="rId47"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A212"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="F212" sqref="F212"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A29" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A30" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A31" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A32" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A37" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A38" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A39" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A40" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A41" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A42" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A43" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A44" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A45" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A46" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A47" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A48" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A49" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A50" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A51" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A52" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A53" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A54" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A55" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A56" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A57" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A58" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A59" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A60" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A61" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A62" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A63" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A64" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A65" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A66" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A67" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A68" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A69" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A70" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A71" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A72" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A73" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A74" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A75" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A76" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A77" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A78" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A79" s="3" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A80" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A81" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A82" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A83" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A84" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A85" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A86" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A87" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A88" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A89" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A90" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A91" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A92" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A93" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A94" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A95" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A96" s="2" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A97" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A98" s="2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A99" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A100" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A101" s="2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A102" s="2" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A103" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A104" s="2" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A105" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A106" s="3" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A107" s="2" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A108" s="2" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A109" s="2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A110" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A111" s="2" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A112" s="2" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A113" s="2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A114" s="2" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A115" s="2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A116" s="2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A117" s="2" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A118" s="2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A119" s="2" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A120" s="2" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A121" s="2" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A122" s="2" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A123" s="2" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A124" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A125" s="2" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A126" s="2" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A127" s="3" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A128" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A129" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A130" s="2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A131" s="2" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A132" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A133" s="2" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A134" s="3" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A135" s="2" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A136" s="2" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A137" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A138" s="2" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A139" s="3" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A140" s="2" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A141" s="2" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A142" s="2" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A143" s="2" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A144" s="2" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A145" s="2" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A146" s="2" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A147" s="2" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A148" s="2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A149" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A150" s="2" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A151" s="2" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A152" s="2" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A153" s="2" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A154" s="2" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A155" s="2" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A156" s="2" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A157" s="2" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A158" s="2" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A159" s="2" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A160" s="2" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A161" s="2" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A162" s="2" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A163" s="2" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A164" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A165" s="3" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A166" s="2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A167" s="2" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A168" s="2" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A169" s="2" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A170" s="2" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A171" s="2" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A172" s="2" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A173" s="2" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A174" s="2" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A175" s="2" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A176" s="2" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A177" s="2" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A178" s="3" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A179" s="2" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A180" s="2" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A181" s="2" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A182" s="2" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A183" s="2" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A184" s="2" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A185" s="2" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A186" s="3" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A187" s="2" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A188" s="2" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A189" s="2" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A190" s="3" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A191" s="3" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A192" s="2" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A193" s="2" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A194" s="2" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A195" s="2" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A196" s="2" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A197" s="2" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A198" s="2" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A199" s="2" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A200" s="2" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A201" s="2" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A202" s="2" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A203" s="2" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A204" s="2" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A205" s="2" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A206" s="2" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A207" s="3" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A208" s="2" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A209" s="3" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A210" s="2" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A211" s="2" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A212" s="2" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A46" r:id="rId1"/>
+    <hyperlink ref="A55" r:id="rId2"/>
+    <hyperlink ref="A57" r:id="rId3"/>
+    <hyperlink ref="A60" r:id="rId4"/>
+    <hyperlink ref="A79" r:id="rId5"/>
+    <hyperlink ref="A106" r:id="rId6"/>
+    <hyperlink ref="A127" r:id="rId7"/>
+    <hyperlink ref="A134" r:id="rId8"/>
+    <hyperlink ref="A139" r:id="rId9"/>
+    <hyperlink ref="A165" r:id="rId10"/>
+    <hyperlink ref="A178" r:id="rId11"/>
+    <hyperlink ref="A186" r:id="rId12"/>
+    <hyperlink ref="A190" r:id="rId13"/>
+    <hyperlink ref="A191" r:id="rId14"/>
+    <hyperlink ref="A207" r:id="rId15"/>
+    <hyperlink ref="A209" r:id="rId16"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+    <sheetView zoomScale="86" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>

</xml_diff>